<commit_message>
The interpretation of CRS Primal results
</commit_message>
<xml_diff>
--- a/RESULTS.xlsx
+++ b/RESULTS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanhanjun/Desktop/DEA_Modelling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanhanjun/Documents/DEA_Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7CC398-FE4A-8741-A1CF-662E66DFDC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65087730-7608-B14A-8C9F-E041B916A58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="51200" windowHeight="28320" xr2:uid="{CC123D8C-AD6D-B147-A650-7E922EB2FDB2}"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="49500" windowHeight="28300" xr2:uid="{CC123D8C-AD6D-B147-A650-7E922EB2FDB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Malmquist_Index" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
   <si>
     <t>SONY</t>
   </si>
@@ -106,12 +106,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -170,9 +176,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -185,43 +188,22 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -235,6 +217,30 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -570,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA3EC40-0B48-074E-9CC3-7F13BA1F9539}">
-  <dimension ref="C5:I18"/>
+  <dimension ref="C5:I34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="186" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScale="186" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -586,45 +592,45 @@
   <sheetData>
     <row r="5" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>0.65276200861865596</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>9.2570394724449306E-2</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>0.57418857074323004</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>0.90295655502142802</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>0.33897744218850301</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -632,64 +638,64 @@
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C8" s="12"/>
-      <c r="D8" s="8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
+      <c r="C8" s="18"/>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
         <v>0.58953838000000003</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C9" s="13"/>
-      <c r="D9" s="9">
+      <c r="C9" s="19"/>
+      <c r="D9" s="8">
         <v>0.65276200861865596</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>9.2570394724449306E-2</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>0.57418857074323004</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>0.90295655502142802</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>0.57498791204824196</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>0.73390852258505102</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="24">
         <v>10.2176978471783</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>0.92281226551464701</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>0.990664674126565</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>1.3406389884290699</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -697,64 +703,64 @@
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C11" s="12"/>
-      <c r="D11" s="8">
-        <v>1</v>
-      </c>
-      <c r="E11" s="8">
-        <v>1</v>
-      </c>
-      <c r="F11" s="8">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8">
-        <v>1</v>
-      </c>
-      <c r="H11" s="8">
+      <c r="C11" s="18"/>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
         <v>1.6962424057955301</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C12" s="13"/>
-      <c r="D12" s="9">
+      <c r="C12" s="19"/>
+      <c r="D12" s="8">
         <v>0.73390852258505102</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>10.2176978471783</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>0.92281226551464701</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>0.990664674126565</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>0.79035813740331295</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>0.99933579533074901</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>0.70588432459056705</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>0.85516210242489199</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <v>1.0893515836619601</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>0.96788056568359504</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -762,118 +768,406 @@
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C14" s="15"/>
-      <c r="D14" s="8">
-        <v>1</v>
-      </c>
-      <c r="E14" s="8">
-        <v>1</v>
-      </c>
-      <c r="F14" s="8">
-        <v>1</v>
-      </c>
-      <c r="G14" s="8">
-        <v>1</v>
-      </c>
-      <c r="H14" s="8">
-        <v>1</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="C14" s="21"/>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1</v>
+      </c>
+      <c r="G14" s="7">
+        <v>1</v>
+      </c>
+      <c r="H14" s="7">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C15" s="16"/>
-      <c r="D15" s="9">
+      <c r="C15" s="22"/>
+      <c r="D15" s="8">
         <v>0.99933579533074901</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>0.70588432459056705</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>0.85516210242489199</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <v>1.0893515836619601</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <v>0.96788056568359504</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>6.5839808739677902E-2</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>1.6691315996662599</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <v>0.75339492189634405</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>0.92763835884319101</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <v>0.87164121503813596</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C17" s="15"/>
-      <c r="D17" s="8">
-        <v>1</v>
-      </c>
-      <c r="E17" s="8">
-        <v>1</v>
-      </c>
-      <c r="F17" s="8">
-        <v>1</v>
-      </c>
-      <c r="G17" s="8">
+      <c r="C17" s="21"/>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7">
         <v>0.99328205999999997</v>
       </c>
-      <c r="H17" s="8">
-        <v>1</v>
-      </c>
-      <c r="I17" s="3" t="s">
+      <c r="H17" s="7">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="17"/>
-      <c r="D18" s="10">
+      <c r="C18" s="23"/>
+      <c r="D18" s="9">
         <v>6.5839808739677902E-2</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <v>1.6691315996662599</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="9">
         <v>0.75339492189634405</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="9">
         <v>0.933912325813265</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="9">
         <v>0.87164121503813596</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="5" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="21" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.639306713634887</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.91396774222579402</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.90984561602054104</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1.09264825176533</v>
+      </c>
+      <c r="H23" s="6">
+        <v>0.34197695844958398</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C24" s="18"/>
+      <c r="D24" s="7">
+        <v>1.000000003849</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.99999999579999999</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1.0000000032859999</v>
+      </c>
+      <c r="G24" s="7">
+        <v>1.0000000006749901</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0.58953837972496803</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C25" s="19"/>
+      <c r="D25" s="8">
+        <v>0.63930671117419602</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0.91396774606445896</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.90984561303078904</v>
+      </c>
+      <c r="G25" s="8">
+        <v>1.0926482510277999</v>
+      </c>
+      <c r="H25" s="8">
+        <v>0.58007581899777805</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C26" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.81644293737885498</v>
+      </c>
+      <c r="E26" s="24">
+        <v>0.93241917593573298</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.92981807497973601</v>
+      </c>
+      <c r="G26" s="6">
+        <v>1.03153551585075</v>
+      </c>
+      <c r="H26" s="6">
+        <v>2.7445289017786298</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C27" s="18"/>
+      <c r="D27" s="7">
+        <v>0.99999999170700005</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.99999997239999905</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1.000000012731</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0.99999999152800001</v>
+      </c>
+      <c r="H27" s="7">
+        <v>1.6962423755032101</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C28" s="19"/>
+      <c r="D28" s="8">
+        <v>0.81644294414961605</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0.93241920167050296</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.92981806314222304</v>
+      </c>
+      <c r="G28" s="8">
+        <v>1.03153552458992</v>
+      </c>
+      <c r="H28" s="8">
+        <v>1.6180051515128699</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C29" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1.0114002473096499</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0.73056562977861605</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0.897764254229381</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0.99340098165344703</v>
+      </c>
+      <c r="H29" s="6">
+        <v>0.90733103299207396</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C30" s="21"/>
+      <c r="D30" s="7">
+        <v>1.000000017616</v>
+      </c>
+      <c r="E30" s="7">
+        <v>1.0000000339999999</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0.99999998822000002</v>
+      </c>
+      <c r="G30" s="7">
+        <v>0.99999999344199897</v>
+      </c>
+      <c r="H30" s="7">
+        <v>1.0000000525170001</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C31" s="22"/>
+      <c r="D31" s="8">
+        <v>1.0114002294928199</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0.73056560493938505</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.89776426480504401</v>
+      </c>
+      <c r="G31" s="8">
+        <v>0.99340098816817102</v>
+      </c>
+      <c r="H31" s="8">
+        <v>0.90733098534177203</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C32" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="7">
+        <v>6.9734009796208293E-2</v>
+      </c>
+      <c r="E32" s="7">
+        <v>1.53221053613608</v>
+      </c>
+      <c r="F32" s="7">
+        <v>0.87871844348871997</v>
+      </c>
+      <c r="G32" s="7">
+        <v>1.0349806088711699</v>
+      </c>
+      <c r="H32" s="7">
+        <v>0.98739715505908299</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C33" s="21"/>
+      <c r="D33" s="7">
+        <v>0.99999999699799902</v>
+      </c>
+      <c r="E33" s="7">
+        <v>1.0000000205999899</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0.99999999729800004</v>
+      </c>
+      <c r="G33" s="7">
+        <v>0.993282046604404</v>
+      </c>
+      <c r="H33" s="7">
+        <v>0.99999996553199999</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="23"/>
+      <c r="D34" s="9">
+        <v>6.9734010005549796E-2</v>
+      </c>
+      <c r="E34" s="9">
+        <v>1.53221050457254</v>
+      </c>
+      <c r="F34" s="9">
+        <v>0.87871844586301795</v>
+      </c>
+      <c r="G34" s="9">
+        <v>1.0419805858862701</v>
+      </c>
+      <c r="H34" s="9">
+        <v>0.98739718909268903</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C34"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C23:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -895,120 +1189,120 @@
   <sheetData>
     <row r="5" spans="5:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E6" s="18"/>
-      <c r="F6" s="18">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10">
         <v>2023</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="10">
         <v>2022</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="10">
         <v>2021</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="10">
         <v>2020</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="10">
         <v>2019</v>
       </c>
     </row>
     <row r="7" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="16">
         <v>0.99999999463536304</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="16">
         <v>0.999999999992085</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="16">
         <v>0.99999999998113698</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="16">
         <v>0.76189817065076904</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="16">
         <v>0.67242510730555105</v>
       </c>
     </row>
     <row r="8" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="12">
         <v>0.16827832149921701</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="12">
         <v>0.99999999994730104</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="12">
         <v>0.340361123502254</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="12">
         <v>0.99999999993285804</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="12">
         <v>0.39139999922832902</v>
       </c>
     </row>
     <row r="9" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="12">
         <v>0.99999999974414799</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="12">
         <v>0.83451410424715899</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="12">
         <v>0.69210263326427501</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="12">
         <v>0.63452493796200005</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="12">
         <v>0.36029787950706099</v>
       </c>
     </row>
     <row r="10" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="12">
         <v>0.76400049236023804</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="12">
         <v>0.57171981801551497</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="12">
         <v>0.99999999872646805</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="12">
         <v>0.66964285606220597</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="12">
         <v>0.758960600225141</v>
       </c>
     </row>
     <row r="11" spans="5:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="14">
         <v>0.99999999999159295</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="14">
         <v>0.96320550194322696</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="14">
         <v>0.99999999999019595</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="14">
         <v>0.24509257169947801</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="14">
         <v>0.25734717499360799</v>
       </c>
     </row>

</xml_diff>